<commit_message>
Update Shaper file with mapping info
1) Comments added to the mappings between shapes --> ontologies
2) New spreadsheet with information about the mappings between ontologies --> shapes
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX360CAK\Documents\DOCTORADO\Tesis\code\Astrea\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7D5097-BCC3-4867-9BCB-89240DC6CC3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13660" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
+    <sheet name="ONTO-SHAPE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="112">
   <si>
     <t>Shape</t>
   </si>
@@ -130,13 +137,267 @@
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>entiendo que es para permitir la reutilización, pero habra casos de uso donde algunas shapes reutilizadas no sean aplicables, por lo que se pueden "desactivar" y el validador no las deberia pillas.  En caso de que se desactiven el valor sería true, asi que por defecto entiendo que false está bien</t>
+  </si>
+  <si>
+    <t>por defecto yo diria que true, aunque luego se pueda modificar</t>
+  </si>
+  <si>
+    <t>aquí hay varias opciones: 
+1) de la propia cardinalidad owl:cardinality / owl:mincardinality/owl:maxcardinality
+2) owl:someValuesFrom se podría tener en cuetna como un min 1</t>
+  </si>
+  <si>
+    <t>si una clase puede tener</t>
+  </si>
+  <si>
+    <t>Axiom</t>
+  </si>
+  <si>
+    <t>owl:allValuesFrom</t>
+  </si>
+  <si>
+    <t>owl:someValuesFrom</t>
+  </si>
+  <si>
+    <t>creo que esto es a nivel de dato y no nos interesa por ahora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:intersectionOf </t>
+  </si>
+  <si>
+    <t>owl:UnionOf</t>
+  </si>
+  <si>
+    <t>owl:complementOf</t>
+  </si>
+  <si>
+    <t>owl:disjointWith</t>
+  </si>
+  <si>
+    <t>owl:cardinality</t>
+  </si>
+  <si>
+    <t>owl:maxCardinality</t>
+  </si>
+  <si>
+    <t>owl:minCardinality</t>
+  </si>
+  <si>
+    <t>rdfs:Class</t>
+  </si>
+  <si>
+    <t>rdfs:domain</t>
+  </si>
+  <si>
+    <t>rdfs:range</t>
+  </si>
+  <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>rdfs:subPropertyOf</t>
+  </si>
+  <si>
+    <t>rdf:type</t>
+  </si>
+  <si>
+    <t>rdfs:Datatype</t>
+  </si>
+  <si>
+    <t>rdf:Property</t>
+  </si>
+  <si>
+    <t>rdfs:subclassOf</t>
+  </si>
+  <si>
+    <t>owl:Individual</t>
+  </si>
+  <si>
+    <t>owl:EquivalentClass</t>
+  </si>
+  <si>
+    <t>owl:EquivalentProperty</t>
+  </si>
+  <si>
+    <t>owl:sameAs</t>
+  </si>
+  <si>
+    <t>owl:differentFrom</t>
+  </si>
+  <si>
+    <t>owl:AllDifferent</t>
+  </si>
+  <si>
+    <t>owl:distinctMembers</t>
+  </si>
+  <si>
+    <t>owl:ObjectProperty</t>
+  </si>
+  <si>
+    <t>owl:DatatypeProperty</t>
+  </si>
+  <si>
+    <t>owl:InverseOf</t>
+  </si>
+  <si>
+    <t>owl:TransitiveProperty</t>
+  </si>
+  <si>
+    <t>owl:SymmetricProperty</t>
+  </si>
+  <si>
+    <t>owl:FunctionalProperty</t>
+  </si>
+  <si>
+    <t>owl:InverseFunctionalProperty</t>
+  </si>
+  <si>
+    <t>owl:Restriction</t>
+  </si>
+  <si>
+    <t>owl:onProperty</t>
+  </si>
+  <si>
+    <t>rdfs:seeAlso</t>
+  </si>
+  <si>
+    <t>rdfs:isDefinedBy</t>
+  </si>
+  <si>
+    <t>owl:AnnotationProperty</t>
+  </si>
+  <si>
+    <t>owl:OntologyProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:minCount  + sh:maxCount ??? </t>
+  </si>
+  <si>
+    <t>sh:NodeShape</t>
+  </si>
+  <si>
+    <t>sh:Property</t>
+  </si>
+  <si>
+    <t>sh:datatype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:Property + sh:datatype	</t>
+  </si>
+  <si>
+    <t>sh:disjoint</t>
+  </si>
+  <si>
+    <t>sh:equals</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>sh:minCount 0 / sh:qualifiedMinCount</t>
+  </si>
+  <si>
+    <t>sh:minCount 1  /sh:qualifiedMinCount</t>
+  </si>
+  <si>
+    <t>sh:minCount /  sh:qualifiedMinCount</t>
+  </si>
+  <si>
+    <t>sh:maxCount /  sh:qualifiedMaxCount</t>
+  </si>
+  <si>
+    <t>no entiendo muy bien lo de qualified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:not </t>
+  </si>
+  <si>
+    <t>creo que se niega una property shape, el mapping no es directo</t>
+  </si>
+  <si>
+    <t>sh:and</t>
+  </si>
+  <si>
+    <t>lo mismo que con sh:not</t>
+  </si>
+  <si>
+    <t>rdfs:Resource</t>
+  </si>
+  <si>
+    <t>rdfs:label /sh:name</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sh:class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sh:node</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:in</t>
+  </si>
+  <si>
+    <t>pero no es exacamente lo mismo, shapes son listas</t>
+  </si>
+  <si>
+    <t>a nivel de instancias, creo que no nos interesa</t>
+  </si>
+  <si>
+    <t>esto se puede añadir tal cual a las shapes</t>
+  </si>
+  <si>
+    <t>no se hasta que punto esto podemos hacerlo, porque si estamos sacandolo de la ontología no van a ser inconsistencias nunca (violation)</t>
+  </si>
+  <si>
+    <t>esto entiendo que es ad-hoc, no automatico</t>
+  </si>
+  <si>
+    <t>creo que no hay mapping directo con ontologías</t>
+  </si>
+  <si>
+    <t>no creo que esto podamos sacarlo de la ontología</t>
+  </si>
+  <si>
+    <t>Annotation properties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,8 +431,46 @@
       <color theme="9"/>
       <name val="Calibri (Cuerpo)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +501,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -242,12 +547,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,6 +565,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -296,6 +610,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -620,249 +942,290 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="54.83203125" customWidth="1"/>
+    <col min="5" max="5" width="33.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:5">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="16">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="16">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="2"/>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="2"/>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="139.5">
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="2"/>
+      <c r="E6" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="2"/>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="2" t="s">
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="2"/>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="2"/>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="16">
-      <c r="A12" s="2"/>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="2"/>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="93">
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="2" t="s">
+      <c r="E13" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="16">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:5">
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="16">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:5">
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="16">
-      <c r="A19" s="2"/>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16">
-      <c r="A20" s="2"/>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="6" customHeight="1">
-      <c r="A21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
-      <c r="A22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
-      <c r="A26" s="7"/>
+    <row r="21" spans="1:5" ht="23" customHeight="1">
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="A26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -871,11 +1234,373 @@
     <mergeCell ref="A14:A20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A530892E-7E9D-4FD9-9FD8-2EAFD3B08BE7}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="52.58203125" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="11"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="13"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="11"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{6B92DA98-1786-42D1-9A4E-D2370C78DEB9}"/>
+    <hyperlink ref="A39" r:id="rId2" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{5183797D-29C3-42FD-850E-40C3AE3D6D8F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some new sh properties included
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX360CAK\Documents\DOCTORADO\Tesis\code\Astrea\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7D5097-BCC3-4867-9BCB-89240DC6CC3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37760" windowHeight="19240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="114">
   <si>
     <t>Shape</t>
   </si>
@@ -392,12 +386,18 @@
   <si>
     <t>Annotation properties</t>
   </si>
+  <si>
+    <t>sh:nodeKind</t>
+  </si>
+  <si>
+    <t>Si vacio poner como string, como sacarlo para un SH:PropertyShape</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,7 +470,7 @@
       <name val="Calibri (Cuerpo)"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -547,7 +553,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -565,9 +571,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -577,6 +580,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -942,34 +949,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
     <col min="4" max="4" width="54.83203125" customWidth="1"/>
-    <col min="5" max="5" width="33.4140625" customWidth="1"/>
+    <col min="5" max="5" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -980,8 +987,8 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="7"/>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -992,8 +999,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="7"/>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1005,8 +1012,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1018,8 +1025,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="139.5">
-      <c r="A6" s="7"/>
+    <row r="6" spans="1:5" ht="75">
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1029,12 +1036,12 @@
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1046,21 +1053,21 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="7"/>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1074,8 +1081,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="15"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1087,8 +1094,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1100,8 +1107,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1113,8 +1120,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="93">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:5" ht="60">
+      <c r="A13" s="15"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1122,12 +1129,12 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:5" ht="16">
+      <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1138,8 +1145,8 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" s="15"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1148,8 +1155,8 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1160,8 +1167,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" s="15"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1172,8 +1179,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1185,8 +1192,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" s="15"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1198,8 +1205,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="15"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1210,7 +1217,7 @@
     </row>
     <row r="21" spans="1:5" ht="23" customHeight="1">
       <c r="A21" s="6"/>
-      <c r="B21" s="9"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="6"/>
@@ -1234,7 +1241,6 @@
     <mergeCell ref="A14:A20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1244,24 +1250,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A530892E-7E9D-4FD9-9FD8-2EAFD3B08BE7}">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="52.58203125" customWidth="1"/>
+    <col min="1" max="1" width="52.5" customWidth="1"/>
     <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1269,7 +1276,7 @@
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1277,7 +1284,7 @@
       <c r="A3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1285,13 +1292,13 @@
       <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1299,19 +1306,19 @@
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
@@ -1328,6 +1335,9 @@
       <c r="B10" t="s">
         <v>86</v>
       </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -1376,182 +1386,176 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>103</v>
+        <v>48</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>98</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="B24" s="10"/>
       <c r="C24" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="B25" s="10"/>
       <c r="C25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B26" s="10"/>
       <c r="C26" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>85</v>
+        <v>69</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="11"/>
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="11"/>
+        <v>72</v>
+      </c>
+      <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="11"/>
+        <v>73</v>
+      </c>
+      <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="13"/>
+        <v>76</v>
+      </c>
+      <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="12"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="13"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="10" t="s">
+      <c r="B36" s="12"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="9" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
       </c>
       <c r="C40" t="s">
         <v>106</v>
@@ -1559,10 +1563,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="C41" t="s">
         <v>106</v>
@@ -1570,10 +1574,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="C42" t="s">
         <v>106</v>
@@ -1581,10 +1585,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="C43" t="s">
         <v>106</v>
@@ -1592,15 +1596,31 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="11"/>
+      <c r="B45" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{6B92DA98-1786-42D1-9A4E-D2370C78DEB9}"/>
-    <hyperlink ref="A39" r:id="rId2" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{5183797D-29C3-42FD-850E-40C3AE3D6D8F}"/>
+    <hyperlink ref="A8" r:id="rId1" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
+    <hyperlink ref="A40" r:id="rId2" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update mappings with spin documentation
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX360CAK\Documents\DOCTORADO\Tesis\code\Astrea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D8E98-EE53-4B7E-A520-31EC728E850A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61349CF-D7A3-4B4D-8EDD-1C637CC8BC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
     <sheet name="ONTO-SHAPE" sheetId="2" r:id="rId2"/>
+    <sheet name="Onto-shape with spin docs" sheetId="3" r:id="rId3"/>
+    <sheet name="Shape-onto with spin docs" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,8 +27,37 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={917CECBB-EFC6-4563-9C1D-EE519962FF49}</author>
+    <author>tc={55D55B28-10D5-458C-8AAA-BD5E74C44BC9}</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    esta traduccion no es directa, en uno se aplica a clases y en shacl a properties
+Respuesta:
+    y lo mismo con intersection y union</t>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="1" shapeId="0" xr:uid="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="237">
   <si>
     <t>Shape</t>
   </si>
@@ -154,9 +185,6 @@
   </si>
   <si>
     <t>si una clase puede tener</t>
-  </si>
-  <si>
-    <t>Axiom</t>
   </si>
   <si>
     <t>owl:allValuesFrom</t>
@@ -510,13 +538,923 @@
   </si>
   <si>
     <t>no le veo sentido a añadir esto</t>
+  </si>
+  <si>
+    <t>SPARQL</t>
+  </si>
+  <si>
+    <t>Constructs</t>
+  </si>
+  <si>
+    <t>OWL</t>
+  </si>
+  <si>
+    <t>SHACL</t>
+  </si>
+  <si>
+    <t>Value Type Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:datatype</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Cardinality Constraints</t>
+  </si>
+  <si>
+    <t>sh:maxCount</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:minCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:maxCount</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:maxCount 1</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:maxCount 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> on a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:inversePath</t>
+    </r>
+  </si>
+  <si>
+    <t>Value Range Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:minExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:minExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>String-based Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:minLength</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:minLength</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:maxLength</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:maxLength</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:length</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:minLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:maxLength</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:pattern</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:pattern</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>rdf:langRange</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:languageIn</t>
+  </si>
+  <si>
+    <t>Property Pair Constraints</t>
+  </si>
+  <si>
+    <t>owl:equivalentProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:propertyDisjointWith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:AllDisjointProperties</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:inverseOf</t>
+  </si>
+  <si>
+    <t>sh:inversePath/sh:equals</t>
+  </si>
+  <si>
+    <t>dash:subSetOf</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:propertyChainAxiom</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:path</t>
+  </si>
+  <si>
+    <t>Logical Constraints</t>
+  </si>
+  <si>
+    <t>sh:not</t>
+  </si>
+  <si>
+    <t>owl:intersectionOf</t>
+  </si>
+  <si>
+    <t>owl:unionOf</t>
+  </si>
+  <si>
+    <t>sh:or</t>
+  </si>
+  <si>
+    <t>owl:qualifiedMin/MaxCardinality 1</t>
+  </si>
+  <si>
+    <t>sh:xone</t>
+  </si>
+  <si>
+    <t>owl:disjointUnionOf</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:node</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:not</t>
+    </r>
+  </si>
+  <si>
+    <t>Shape-based (structural) Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>rdfs:subClassOf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:equivalentClass</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:node</t>
+  </si>
+  <si>
+    <t>sh:property</t>
+  </si>
+  <si>
+    <t>sh:qualifiedMinCount 1 or dash:hasValueWithClass</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:qualifiedMinCardinality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:qualifiedMinCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>Other Constraints</t>
+  </si>
+  <si>
+    <t>sh:hasValue</t>
+  </si>
+  <si>
+    <t>owl:oneOf</t>
+  </si>
+  <si>
+    <t>owl:ReflexiveProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:disjoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in a node shape</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:IrreflexiveProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:disjoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in a node shape</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:AsymmetricProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> operator</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:hasKey</t>
+  </si>
+  <si>
+    <t>dash:uriStart</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:sameAs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:differentFrom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:AllDifferent</t>
+    </r>
+  </si>
+  <si>
+    <t>Missing constructs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:complementOf	</t>
+  </si>
+  <si>
+    <t>owl:minCardinality, owl:maxCardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> String-based Constraints</t>
+  </si>
+  <si>
+    <t>Property Pair  Constraints</t>
+  </si>
+  <si>
+    <t>Logical Constraint  Constraints</t>
+  </si>
+  <si>
+    <t>Shape-based  Constraints</t>
+  </si>
+  <si>
+    <t>Other Constraint</t>
+  </si>
+  <si>
+    <t>sh:closed, sh:ignoredProperties</t>
+  </si>
+  <si>
+    <t>owl:Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:class </t>
+  </si>
+  <si>
+    <t>sh:datatype : rdfs:Resource</t>
+  </si>
+  <si>
+    <t>owl:Datatype</t>
+  </si>
+  <si>
+    <t>xsd:anyURI, xsd:string</t>
+  </si>
+  <si>
+    <t>Non-Validating Property Shape Characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:name </t>
+  </si>
+  <si>
+    <t>sh:description</t>
+  </si>
+  <si>
+    <t>sh:order</t>
+  </si>
+  <si>
+    <t>sh:group</t>
+  </si>
+  <si>
+    <t>sh:defaultValue</t>
+  </si>
+  <si>
+    <t>Other Characteristics</t>
+  </si>
+  <si>
+    <t>rdfs:Property</t>
+  </si>
+  <si>
+    <t>sh:qualifiedValueShape, sh:qualifiedMinCount, sh:qualifiedMaxCount :  xsd:integer</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:qualifiedMinCardinality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>QUERY</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?dataProperty;
+    sh:datatype ?datatype ;
+ ]
+} WHERE{
+             ?type a owl:Class .
+	OPTIONAL { 
+		?dataProperty a owl:DatatypeProperty ;
+		rdfs:domain ?type ;
+		rdfs:range ?datatype .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?objectProperty;
+    sh:class ?typeInRange ;
+ ]
+} WHERE{
+?type a owl:Class .
+	OPTIONAL { 
+		?objectProperty a owl:ObjectProperty  ;
+		rdfs:domain ?type ;
+		rdfs:range ?typeInRange .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type
+} WHERE
+              ?type a owl:Class .
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:name  ?shapeNodeName; 
+} WHERE{
+    ?type a owl:Class .
+	OPTIONAL { ?type rdfs:label ?shapeNodeName . }
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:description  ?shapeNodeName; 
+} WHERE{
+    ?type a owl:Class .
+    OPTIONAL { ?type rdfs:comment ?shapeNodeComment .} 
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?objectProperty;
+    sh:class ?typeInRange ;
+ ]
+} WHERE{
+	OPTIONAL { 
+		?objectProperty a owl:ObjectProperty  ;
+		rdfs:range ?typeInRange .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>QUERY (aunque la query es mejor solo en la hoja siguiente)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -588,8 +1526,45 @@
       <color theme="1"/>
       <name val="Calibri (Cuerpo)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,10 +1607,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -672,7 +1662,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -700,10 +1690,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -746,6 +1764,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Alba Fernandez Izquierdo" id="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" userId="0420dbf024001011" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,12 +2092,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A25" dT="2019-10-21T14:31:05.31" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+    <text>esta traduccion no es directa, en uno se aplica a clases y en shacl a properties</text>
+  </threadedComment>
+  <threadedComment ref="A25" dT="2019-10-21T14:31:16.59" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{4691690A-8526-40CC-8572-4F4A8AA0569D}" parentId="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+    <text>y lo mismo con intersection y union</text>
+  </threadedComment>
+  <threadedComment ref="A31" dT="2019-10-21T14:25:54.99" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
+    <text>Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1096,7 +2134,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1108,7 +2146,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +2158,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1129,11 +2167,11 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1142,11 +2180,11 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="77.5">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +2199,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1170,11 +2208,11 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1183,11 +2221,11 @@
         <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1202,7 +2240,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1215,7 +2253,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1224,11 +2262,11 @@
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1237,11 +2275,11 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="62">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +2292,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1266,7 +2304,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1276,7 +2314,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +2326,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +2338,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1309,11 +2347,11 @@
         <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1322,11 +2360,11 @@
         <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1342,177 +2380,177 @@
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="16"/>
+        <v>125</v>
+      </c>
+      <c r="C26" s="15"/>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="16"/>
+        <v>126</v>
+      </c>
+      <c r="C27" s="15"/>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" t="s">
         <v>117</v>
-      </c>
-      <c r="E32" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="16"/>
+        <v>135</v>
+      </c>
+      <c r="C36" s="15"/>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="16"/>
+        <v>136</v>
+      </c>
+      <c r="C38" s="15"/>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="16"/>
+        <v>137</v>
+      </c>
+      <c r="C39" s="15"/>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="16"/>
+        <v>140</v>
+      </c>
+      <c r="C42" s="15"/>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1532,10 +2570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1545,356 +2583,359 @@
     <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="B10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
       <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="12"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="10"/>
     </row>
@@ -1911,4 +2952,875 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F95036-FCE7-4554-B2BD-5DEBDECE98D2}">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" customWidth="1"/>
+    <col min="3" max="3" width="62.9140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="17" customFormat="1">
+      <c r="A10" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" ht="25">
+      <c r="A11" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="17" customFormat="1">
+      <c r="A12" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="17" customFormat="1">
+      <c r="A18" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="17" customFormat="1">
+      <c r="A24" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="17" customFormat="1" ht="18" customHeight="1">
+      <c r="A30" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="17" customFormat="1">
+      <c r="A35" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="17" customFormat="1">
+      <c r="A47" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A30:C30"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent" xr:uid="{54148F92-94B4-4AF4-B5FA-8D0B4D55E342}"/>
+    <hyperlink ref="B33" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent" xr:uid="{E32B02DA-AF91-4C14-B44F-29469A21821F}"/>
+    <hyperlink ref="B43" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent" xr:uid="{BFB54128-E8D0-4C44-8686-E6193A567A0A}"/>
+    <hyperlink ref="A48" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{50940326-B931-4322-8541-1A1951DAA2DD}"/>
+    <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{03B96900-38DE-4802-916C-94144F0EE515}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46DF551-1B81-469E-97A7-D91ACDB8B622}">
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3" ht="279">
+      <c r="A3" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="310">
+      <c r="A4" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="25">
+      <c r="A5" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="18"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="18"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="18"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3" ht="139.5">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="310">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="18"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="1:3" ht="201.5">
+      <c r="A37" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="201.5">
+      <c r="A38" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="18"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="18"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" s="18"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="18"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="18"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="18"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A21:C21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new approach included, also some test casses. Included file status that reports each of the owl statements that we cover in which unitary test have been tested and what expected sh property they generate
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX360CAK\Documents\DOCTORADO\Tesis\code\Astrea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D8E98-EE53-4B7E-A520-31EC728E850A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61349CF-D7A3-4B4D-8EDD-1C637CC8BC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
     <sheet name="ONTO-SHAPE" sheetId="2" r:id="rId2"/>
+    <sheet name="Onto-shape with spin docs" sheetId="3" r:id="rId3"/>
+    <sheet name="Shape-onto with spin docs" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,8 +27,37 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={917CECBB-EFC6-4563-9C1D-EE519962FF49}</author>
+    <author>tc={55D55B28-10D5-458C-8AAA-BD5E74C44BC9}</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    esta traduccion no es directa, en uno se aplica a clases y en shacl a properties
+Respuesta:
+    y lo mismo con intersection y union</t>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="1" shapeId="0" xr:uid="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="237">
   <si>
     <t>Shape</t>
   </si>
@@ -154,9 +185,6 @@
   </si>
   <si>
     <t>si una clase puede tener</t>
-  </si>
-  <si>
-    <t>Axiom</t>
   </si>
   <si>
     <t>owl:allValuesFrom</t>
@@ -510,13 +538,923 @@
   </si>
   <si>
     <t>no le veo sentido a añadir esto</t>
+  </si>
+  <si>
+    <t>SPARQL</t>
+  </si>
+  <si>
+    <t>Constructs</t>
+  </si>
+  <si>
+    <t>OWL</t>
+  </si>
+  <si>
+    <t>SHACL</t>
+  </si>
+  <si>
+    <t>Value Type Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:datatype</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Cardinality Constraints</t>
+  </si>
+  <si>
+    <t>sh:maxCount</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:minCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:maxCount</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:maxCount 1</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:maxCount 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> on a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:inversePath</t>
+    </r>
+  </si>
+  <si>
+    <t>Value Range Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:minExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:minExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>String-based Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:minLength</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:minLength</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:maxLength</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:maxLength</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:length</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:minLength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:maxLength</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:pattern</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:pattern</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>rdf:langRange</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:languageIn</t>
+  </si>
+  <si>
+    <t>Property Pair Constraints</t>
+  </si>
+  <si>
+    <t>owl:equivalentProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:propertyDisjointWith</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:AllDisjointProperties</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:inverseOf</t>
+  </si>
+  <si>
+    <t>sh:inversePath/sh:equals</t>
+  </si>
+  <si>
+    <t>dash:subSetOf</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:propertyChainAxiom</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:path</t>
+  </si>
+  <si>
+    <t>Logical Constraints</t>
+  </si>
+  <si>
+    <t>sh:not</t>
+  </si>
+  <si>
+    <t>owl:intersectionOf</t>
+  </si>
+  <si>
+    <t>owl:unionOf</t>
+  </si>
+  <si>
+    <t>sh:or</t>
+  </si>
+  <si>
+    <t>owl:qualifiedMin/MaxCardinality 1</t>
+  </si>
+  <si>
+    <t>sh:xone</t>
+  </si>
+  <si>
+    <t>owl:disjointUnionOf</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:node</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:not</t>
+    </r>
+  </si>
+  <si>
+    <t>Shape-based (structural) Constraints</t>
+  </si>
+  <si>
+    <r>
+      <t>rdfs:subClassOf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:equivalentClass</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:node</t>
+  </si>
+  <si>
+    <t>sh:property</t>
+  </si>
+  <si>
+    <t>sh:qualifiedMinCount 1 or dash:hasValueWithClass</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:qualifiedMinCardinality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:qualifiedMinCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>Other Constraints</t>
+  </si>
+  <si>
+    <t>sh:hasValue</t>
+  </si>
+  <si>
+    <t>owl:oneOf</t>
+  </si>
+  <si>
+    <t>owl:ReflexiveProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>sh:disjoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in a node shape</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:IrreflexiveProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:disjoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in a node shape</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:AsymmetricProperty</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> operator</t>
+    </r>
+  </si>
+  <si>
+    <t>owl:hasKey</t>
+  </si>
+  <si>
+    <t>dash:uriStart</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:sameAs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:differentFrom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:AllDifferent</t>
+    </r>
+  </si>
+  <si>
+    <t>Missing constructs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:complementOf	</t>
+  </si>
+  <si>
+    <t>owl:minCardinality, owl:maxCardinality</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> String-based Constraints</t>
+  </si>
+  <si>
+    <t>Property Pair  Constraints</t>
+  </si>
+  <si>
+    <t>Logical Constraint  Constraints</t>
+  </si>
+  <si>
+    <t>Shape-based  Constraints</t>
+  </si>
+  <si>
+    <t>Other Constraint</t>
+  </si>
+  <si>
+    <t>sh:closed, sh:ignoredProperties</t>
+  </si>
+  <si>
+    <t>owl:Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:class </t>
+  </si>
+  <si>
+    <t>sh:datatype : rdfs:Resource</t>
+  </si>
+  <si>
+    <t>owl:Datatype</t>
+  </si>
+  <si>
+    <t>xsd:anyURI, xsd:string</t>
+  </si>
+  <si>
+    <t>Non-Validating Property Shape Characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:name </t>
+  </si>
+  <si>
+    <t>sh:description</t>
+  </si>
+  <si>
+    <t>sh:order</t>
+  </si>
+  <si>
+    <t>sh:group</t>
+  </si>
+  <si>
+    <t>sh:defaultValue</t>
+  </si>
+  <si>
+    <t>Other Characteristics</t>
+  </si>
+  <si>
+    <t>rdfs:Property</t>
+  </si>
+  <si>
+    <t>sh:qualifiedValueShape, sh:qualifiedMinCount, sh:qualifiedMaxCount :  xsd:integer</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:qualifiedMinCardinality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <t>QUERY</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?dataProperty;
+    sh:datatype ?datatype ;
+ ]
+} WHERE{
+             ?type a owl:Class .
+	OPTIONAL { 
+		?dataProperty a owl:DatatypeProperty ;
+		rdfs:domain ?type ;
+		rdfs:range ?datatype .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?objectProperty;
+    sh:class ?typeInRange ;
+ ]
+} WHERE{
+?type a owl:Class .
+	OPTIONAL { 
+		?objectProperty a owl:ObjectProperty  ;
+		rdfs:domain ?type ;
+		rdfs:range ?typeInRange .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type
+} WHERE
+              ?type a owl:Class .
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:name  ?shapeNodeName; 
+} WHERE{
+    ?type a owl:Class .
+	OPTIONAL { ?type rdfs:label ?shapeNodeName . }
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:description  ?shapeNodeName; 
+} WHERE{
+    ?type a owl:Class .
+    OPTIONAL { ?type rdfs:comment ?shapeNodeComment .} 
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>PREFIX owl: &lt;http://www.w3.org/2002/07/owl#&gt; 
+PREFIX rdfs: &lt;http://www.w3.org/2000/01/rdf-schema#&gt; 
+PREFIX sh: &lt;http://www.w3.org/ns/shacl#&gt;
+CONSTRUCT { 
+ ?shapeUrl a sh:NodeShape ;
+ sh:targetClass ?type;
+ sh:property [
+    sh:path ?objectProperty;
+    sh:class ?typeInRange ;
+ ]
+} WHERE{
+	OPTIONAL { 
+		?objectProperty a owl:ObjectProperty  ;
+		rdfs:range ?typeInRange .
+	}
+ 	FILTER (!isBlank(?type)) .
+ 	BIND ( URI(CONCAT(STR(?type),"Shape")) AS ?shapeUrl) .
+}</t>
+  </si>
+  <si>
+    <t>QUERY (aunque la query es mejor solo en la hoja siguiente)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -588,8 +1526,45 @@
       <color theme="1"/>
       <name val="Calibri (Cuerpo)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,10 +1607,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -672,7 +1662,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -700,10 +1690,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -746,6 +1764,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Alba Fernandez Izquierdo" id="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" userId="0420dbf024001011" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1068,12 +2092,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A25" dT="2019-10-21T14:31:05.31" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+    <text>esta traduccion no es directa, en uno se aplica a clases y en shacl a properties</text>
+  </threadedComment>
+  <threadedComment ref="A25" dT="2019-10-21T14:31:16.59" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{4691690A-8526-40CC-8572-4F4A8AA0569D}" parentId="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+    <text>y lo mismo con intersection y union</text>
+  </threadedComment>
+  <threadedComment ref="A31" dT="2019-10-21T14:25:54.99" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
+    <text>Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1096,7 +2134,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1108,7 +2146,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +2158,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1129,11 +2167,11 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1142,11 +2180,11 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="77.5">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +2199,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1170,11 +2208,11 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1183,11 +2221,11 @@
         <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1202,7 +2240,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1215,7 +2253,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1224,11 +2262,11 @@
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1237,11 +2275,11 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="62">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +2292,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1266,7 +2304,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1276,7 +2314,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1288,7 +2326,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +2338,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1309,11 +2347,11 @@
         <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1322,11 +2360,11 @@
         <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1342,177 +2380,177 @@
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="16"/>
+        <v>125</v>
+      </c>
+      <c r="C26" s="15"/>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="16"/>
+        <v>126</v>
+      </c>
+      <c r="C27" s="15"/>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" t="s">
         <v>117</v>
-      </c>
-      <c r="E32" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C36" s="16"/>
+        <v>135</v>
+      </c>
+      <c r="C36" s="15"/>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="16"/>
+        <v>136</v>
+      </c>
+      <c r="C38" s="15"/>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" s="16"/>
+        <v>137</v>
+      </c>
+      <c r="C39" s="15"/>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="16"/>
+        <v>140</v>
+      </c>
+      <c r="C42" s="15"/>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1532,10 +2570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1545,356 +2583,359 @@
     <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>42</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="B10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="10"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
       <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="10"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="10"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="12"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="C40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="10"/>
     </row>
@@ -1911,4 +2952,875 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F95036-FCE7-4554-B2BD-5DEBDECE98D2}">
+  <dimension ref="A1:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" customWidth="1"/>
+    <col min="3" max="3" width="62.9140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="17" customFormat="1">
+      <c r="A10" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" ht="25">
+      <c r="A11" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="17" customFormat="1">
+      <c r="A12" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="17" customFormat="1">
+      <c r="A18" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="17" customFormat="1">
+      <c r="A24" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="17" customFormat="1" ht="18" customHeight="1">
+      <c r="A30" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="17" customFormat="1">
+      <c r="A35" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="17" customFormat="1">
+      <c r="A47" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A30:C30"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent" xr:uid="{54148F92-94B4-4AF4-B5FA-8D0B4D55E342}"/>
+    <hyperlink ref="B33" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent" xr:uid="{E32B02DA-AF91-4C14-B44F-29469A21821F}"/>
+    <hyperlink ref="B43" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent" xr:uid="{BFB54128-E8D0-4C44-8686-E6193A567A0A}"/>
+    <hyperlink ref="A48" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{50940326-B931-4322-8541-1A1951DAA2DD}"/>
+    <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{03B96900-38DE-4802-916C-94144F0EE515}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46DF551-1B81-469E-97A7-D91ACDB8B622}">
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="48.83203125" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:3" ht="279">
+      <c r="A3" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="310">
+      <c r="A4" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="25">
+      <c r="A5" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="18"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="18"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="18"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3" ht="139.5">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="310">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="18"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="1:3" ht="201.5">
+      <c r="A37" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="201.5">
+      <c r="A38" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B39" s="18"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B40" s="18"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B41" s="18"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="18"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="18"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="18"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A21:C21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new shacl properties included
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UX360CAK\Documents\DOCTORADO\Tesis\code\Astrea\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61349CF-D7A3-4B4D-8EDD-1C637CC8BC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -28,28 +22,46 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={917CECBB-EFC6-4563-9C1D-EE519962FF49}</author>
     <author>tc={55D55B28-10D5-458C-8AAA-BD5E74C44BC9}</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
+    <comment ref="A25" authorId="0">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     esta traduccion no es directa, en uno se aplica a clases y en shacl a properties
 Respuesta:
     y lo mismo con intersection y union</t>
+        </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="1" shapeId="0" xr:uid="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
+    <comment ref="A31" authorId="1">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -57,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="241">
   <si>
     <t>Shape</t>
   </si>
@@ -1449,12 +1461,24 @@
   <si>
     <t>QUERY (aunque la query es mejor solo en la hoja siguiente)</t>
   </si>
+  <si>
+    <t>AnnotationPropertiesTest</t>
+  </si>
+  <si>
+    <t>FilledInformationTest</t>
+  </si>
+  <si>
+    <t>CardinalityTest</t>
+  </si>
+  <si>
+    <t>PropertyCharacteristicsTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1558,10 +1582,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1662,7 +1685,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1691,20 +1714,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1721,6 +1735,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -1764,12 +1792,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Alba Fernandez Izquierdo" id="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" userId="0420dbf024001011" providerId="Windows Live"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2092,37 +2114,23 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A25" dT="2019-10-21T14:31:05.31" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
-    <text>esta traduccion no es directa, en uno se aplica a clases y en shacl a properties</text>
-  </threadedComment>
-  <threadedComment ref="A25" dT="2019-10-21T14:31:16.59" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{4691690A-8526-40CC-8572-4F4A8AA0569D}" parentId="{917CECBB-EFC6-4563-9C1D-EE519962FF49}">
-    <text>y lo mismo con intersection y union</text>
-  </threadedComment>
-  <threadedComment ref="A31" dT="2019-10-21T14:25:54.99" personId="{4DB8A029-A1A9-4C70-B665-A77A5DED7782}" id="{55D55B28-10D5-458C-8AAA-BD5E74C44BC9}">
-    <text>Entiendo que esto implica que una subclassOf genera una nueva shape, pero no estoy muy convencida de esto a nivel de generacion</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView topLeftCell="B18" workbookViewId="0">
       <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.25" customWidth="1"/>
+    <col min="4" max="4" width="43.1640625" customWidth="1"/>
     <col min="5" max="5" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16">
       <c r="A1" s="1"/>
       <c r="B1" s="13" t="s">
         <v>8</v>
@@ -2133,8 +2141,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2145,8 +2153,8 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="16"/>
+    <row r="3" spans="1:5" ht="16">
+      <c r="A3" s="29"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2157,8 +2165,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="16"/>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="29"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2170,8 +2178,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="29"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2183,8 +2191,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="77.5">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:5" ht="75">
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2198,8 +2206,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:5" ht="16">
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2211,8 +2219,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="16"/>
+    <row r="8" spans="1:5" ht="16">
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2224,8 +2232,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:5" ht="16">
+      <c r="A9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2239,8 +2247,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:5" ht="16">
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2252,8 +2260,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="16"/>
+    <row r="11" spans="1:5" ht="16">
+      <c r="A11" s="29"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2265,8 +2273,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="16"/>
+    <row r="12" spans="1:5" ht="16">
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2278,8 +2286,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="62">
-      <c r="A13" s="16"/>
+    <row r="13" spans="1:5" ht="60">
+      <c r="A13" s="29"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2291,8 +2299,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:5" ht="16">
+      <c r="A14" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2303,8 +2311,8 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="16"/>
+    <row r="15" spans="1:5" ht="16">
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2313,8 +2321,8 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="16"/>
+    <row r="16" spans="1:5" ht="16">
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2325,8 +2333,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="16"/>
+    <row r="17" spans="1:5" ht="16">
+      <c r="A17" s="29"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2337,8 +2345,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="16"/>
+    <row r="18" spans="1:5" ht="16">
+      <c r="A18" s="29"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2350,8 +2358,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="16"/>
+    <row r="19" spans="1:5" ht="16">
+      <c r="A19" s="29"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2363,8 +2371,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:5" ht="16">
+      <c r="A20" s="29"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2415,7 +2423,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16">
       <c r="B27" s="1" t="s">
         <v>126</v>
       </c>
@@ -2424,7 +2432,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="16">
       <c r="B28" s="1" t="s">
         <v>127</v>
       </c>
@@ -2433,7 +2441,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="16">
       <c r="B29" s="1" t="s">
         <v>128</v>
       </c>
@@ -2442,7 +2450,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="16">
       <c r="B30" s="1" t="s">
         <v>129</v>
       </c>
@@ -2451,7 +2459,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="16">
       <c r="B31" s="1" t="s">
         <v>130</v>
       </c>
@@ -2460,7 +2468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="16">
       <c r="B32" s="1" t="s">
         <v>131</v>
       </c>
@@ -2472,7 +2480,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" ht="16">
       <c r="B33" s="1" t="s">
         <v>132</v>
       </c>
@@ -2481,7 +2489,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" ht="16">
       <c r="B34" s="1" t="s">
         <v>133</v>
       </c>
@@ -2493,7 +2501,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" ht="16">
       <c r="B35" s="1" t="s">
         <v>134</v>
       </c>
@@ -2505,7 +2513,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" ht="16">
       <c r="B36" s="1" t="s">
         <v>135</v>
       </c>
@@ -2514,7 +2522,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" ht="16">
       <c r="B38" s="1" t="s">
         <v>136</v>
       </c>
@@ -2523,7 +2531,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" ht="16">
       <c r="B39" s="1" t="s">
         <v>137</v>
       </c>
@@ -2532,19 +2540,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" ht="16">
       <c r="B40" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" ht="16">
       <c r="B41" s="1" t="s">
         <v>139</v>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" ht="16">
       <c r="B42" s="1" t="s">
         <v>140</v>
       </c>
@@ -2569,14 +2577,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="52.5" customWidth="1"/>
     <col min="2" max="2" width="60.6640625" customWidth="1"/>
@@ -2941,11 +2949,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A40" r:id="rId2" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A8" r:id="rId1" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
+    <hyperlink ref="A40" r:id="rId2" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2955,471 +2962,499 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F95036-FCE7-4554-B2BD-5DEBDECE98D2}">
-  <dimension ref="A1:C60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
     <col min="2" max="2" width="40.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62.9140625" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="23" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="23" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="26" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
+      <c r="D5" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23" t="s">
+      <c r="D6" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="26" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="23" t="s">
+      <c r="D7" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="26" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="23" t="s">
+      <c r="D8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="17" customFormat="1">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:4" s="16" customFormat="1">
+      <c r="A10" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:3" ht="25">
-      <c r="A11" s="23" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="17" customFormat="1">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:4" s="16" customFormat="1">
+      <c r="A12" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="23" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="20" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="20" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="17" customFormat="1">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:3" s="16" customFormat="1">
+      <c r="A18" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="20" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="20" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="20" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="20" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="20" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="17" customFormat="1">
-      <c r="A24" s="20" t="s">
+    <row r="24" spans="1:3" s="16" customFormat="1">
+      <c r="A24" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="20" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="20" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="20" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="20" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="17" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:3" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="A30" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="20" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="23" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="23" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="20" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="17" customFormat="1">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:4" s="16" customFormat="1">
+      <c r="A35" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="23" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+    </row>
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="26" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="23" t="s">
+      <c r="D36" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="23" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="20" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="23" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="23" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="23" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="20" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="23" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="20" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="23" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="17" customFormat="1">
-      <c r="A47" s="20" t="s">
+    <row r="47" spans="1:4" s="16" customFormat="1">
+      <c r="A47" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="22" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="22" t="s">
+    <row r="49" spans="1:4">
+      <c r="A49" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="22" t="s">
+    <row r="50" spans="1:4" ht="16">
+      <c r="A50" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="22" t="s">
+      <c r="D50" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="16">
+      <c r="A51" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="22" t="s">
+      <c r="D51" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="16">
+      <c r="A52" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="27" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="22" t="s">
+      <c r="D52" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16">
+      <c r="A53" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="22" t="s">
+      <c r="D53" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="22" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="22" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="22" t="s">
+    <row r="57" spans="1:4">
+      <c r="A57" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="22" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="22" t="s">
+    <row r="59" spans="1:4">
+      <c r="A59" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -3440,27 +3475,31 @@
     <mergeCell ref="A30:C30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent" xr:uid="{54148F92-94B4-4AF4-B5FA-8D0B4D55E342}"/>
-    <hyperlink ref="B33" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent" xr:uid="{E32B02DA-AF91-4C14-B44F-29469A21821F}"/>
-    <hyperlink ref="B43" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent" xr:uid="{BFB54128-E8D0-4C44-8686-E6193A567A0A}"/>
-    <hyperlink ref="A48" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain" xr:uid="{50940326-B931-4322-8541-1A1951DAA2DD}"/>
-    <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment" xr:uid="{03B96900-38DE-4802-916C-94144F0EE515}"/>
+    <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent"/>
+    <hyperlink ref="B33" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent"/>
+    <hyperlink ref="B43" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent"/>
+    <hyperlink ref="A48" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
+    <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId6"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46DF551-1B81-469E-97A7-D91ACDB8B622}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48.83203125" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
@@ -3468,61 +3507,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:3" ht="279">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+    </row>
+    <row r="3" spans="1:3" ht="288">
+      <c r="A3" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="310">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:3" ht="300">
+      <c r="A4" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:3" ht="30">
+      <c r="A5" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+    </row>
+    <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -3531,36 +3570,36 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+    </row>
+    <row r="12" spans="1:3" ht="16">
       <c r="A12" s="1" t="s">
         <v>129</v>
       </c>
@@ -3568,7 +3607,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="16">
       <c r="A13" s="1" t="s">
         <v>130</v>
       </c>
@@ -3576,7 +3615,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="16">
       <c r="A14" s="1" t="s">
         <v>131</v>
       </c>
@@ -3584,20 +3623,20 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="16">
       <c r="A15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+    </row>
+    <row r="17" spans="1:3" ht="16">
       <c r="A17" s="1" t="s">
         <v>125</v>
       </c>
@@ -3605,7 +3644,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="16">
       <c r="A18" s="1" t="s">
         <v>126</v>
       </c>
@@ -3613,26 +3652,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="16">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="18"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" ht="16">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+    </row>
+    <row r="22" spans="1:3" ht="16">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
@@ -3640,7 +3679,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="16">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -3648,7 +3687,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" ht="16">
       <c r="A24" s="1" t="s">
         <v>122</v>
       </c>
@@ -3656,7 +3695,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" ht="16">
       <c r="A25" s="1" t="s">
         <v>124</v>
       </c>
@@ -3665,65 +3704,65 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-    </row>
-    <row r="27" spans="1:3" ht="139.5">
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+    </row>
+    <row r="27" spans="1:3" ht="135">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>214</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="310">
+    <row r="28" spans="1:3" ht="300">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>226</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" ht="16">
       <c r="A29" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="19" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+    </row>
+    <row r="32" spans="1:3" ht="16">
+      <c r="A32" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="18"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="19" t="s">
+      <c r="B32" s="17"/>
+    </row>
+    <row r="33" spans="1:3" ht="16">
+      <c r="A33" s="18" t="s">
         <v>194</v>
       </c>
       <c r="B33" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="19" t="s">
+    <row r="34" spans="1:3" ht="16">
+      <c r="A34" s="18" t="s">
         <v>96</v>
       </c>
       <c r="B34" t="s">
@@ -3731,14 +3770,14 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-    </row>
-    <row r="37" spans="1:3" ht="201.5">
-      <c r="A37" s="19" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+    </row>
+    <row r="37" spans="1:3" ht="195">
+      <c r="A37" s="18" t="s">
         <v>220</v>
       </c>
       <c r="B37" t="s">
@@ -3748,8 +3787,8 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="201.5">
-      <c r="A38" s="19" t="s">
+    <row r="38" spans="1:3" ht="195">
+      <c r="A38" s="18" t="s">
         <v>221</v>
       </c>
       <c r="B38" t="s">
@@ -3759,54 +3798,54 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:3" ht="16">
+      <c r="A39" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="18"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="19" t="s">
+      <c r="B39" s="17"/>
+    </row>
+    <row r="40" spans="1:3" ht="16">
+      <c r="A40" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B40" s="18"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="19" t="s">
+      <c r="B40" s="17"/>
+    </row>
+    <row r="41" spans="1:3" ht="16">
+      <c r="A41" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="B41" s="18"/>
+      <c r="B41" s="17"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+    </row>
+    <row r="44" spans="1:3" ht="16">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="18"/>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="B44" s="17"/>
+    </row>
+    <row r="45" spans="1:3" ht="16">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="18"/>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="B45" s="17"/>
+    </row>
+    <row r="46" spans="1:3" ht="16">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="18"/>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="B46" s="17"/>
+    </row>
+    <row r="47" spans="1:3" ht="16">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="18"/>
+      <c r="B47" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3822,5 +3861,10 @@
     <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new owl expressiones covered
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1580" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="244">
   <si>
     <t>Shape</t>
   </si>
@@ -1472,6 +1472,15 @@
   </si>
   <si>
     <t>PropertyCharacteristicsTest</t>
+  </si>
+  <si>
+    <t>rdfs:label / sh:Description</t>
+  </si>
+  <si>
+    <t>sh:PropertyShape</t>
+  </si>
+  <si>
+    <t>RDFSchemaFeaturesTest</t>
   </si>
 </sst>
 </file>
@@ -1655,9 +1664,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1751,7 +1762,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="30">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
@@ -1779,6 +1790,8 @@
     <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2963,10 +2976,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3367,7 +3380,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>56</v>
+        <v>241</v>
       </c>
       <c r="D50" s="28" t="s">
         <v>237</v>
@@ -3423,19 +3436,25 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="19" t="s">
-        <v>84</v>
+      <c r="B56" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D56" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="27" t="s">
         <v>83</v>
+      </c>
+      <c r="D57" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3447,19 +3466,36 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>84</v>
+      <c r="B59" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D59" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" t="s">
+      <c r="A60" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B60" t="s">
-        <v>86</v>
+      <c r="B60" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D61" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3482,6 +3518,7 @@
     <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId6"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
refined tests, new owl coverage included
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <author>tc={55D55B28-10D5-458C-8AAA-BD5E74C44BC9}</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0">
+    <comment ref="A26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="1">
+    <comment ref="A32" authorId="1">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="253">
   <si>
     <t>Shape</t>
   </si>
@@ -977,28 +977,6 @@
   </si>
   <si>
     <t>dash:subSetOf</t>
-  </si>
-  <si>
-    <r>
-      <t>owl:onProperty</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>owl:propertyChainAxiom</t>
-    </r>
   </si>
   <si>
     <t>sh:path</t>
@@ -1481,6 +1459,65 @@
   </si>
   <si>
     <t>RDFSchemaFeaturesTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En este test si una clase esta definida como rdf:Property no se generará ninguna de estas restricciones </t>
+  </si>
+  <si>
+    <t>Comentar esto del domain</t>
+  </si>
+  <si>
+    <t>owl:propertyChainAxiom</t>
+  </si>
+  <si>
+    <r>
+      <t>owl:onProperty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>PropertyRestrictionsTest</t>
+  </si>
+  <si>
+    <t>Esto puede a puntar a un union o algo?</t>
+  </si>
+  <si>
+    <t>EquialityTest</t>
+  </si>
+  <si>
+    <t>Esto se puede encontrar en un owl:Restriction?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sh:class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / sh:datatype / sh:node</t>
+    </r>
+  </si>
+  <si>
+    <t>sh:node apunta a un shape</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1633,7 @@
       <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1645,6 +1682,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1664,7 +1707,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1695,8 +1738,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1752,6 +1800,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1762,7 +1819,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="35">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
@@ -1792,6 +1849,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2155,7 +2217,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2167,7 +2229,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16">
-      <c r="A3" s="29"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2179,7 +2241,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2192,7 +2254,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2205,7 +2267,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="75">
-      <c r="A6" s="29"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2220,7 +2282,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2233,7 +2295,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2246,7 +2308,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2261,7 +2323,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2274,7 +2336,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2287,7 +2349,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="16">
-      <c r="A12" s="29"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2300,7 +2362,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="60">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2313,7 +2375,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="16">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="32" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2325,7 +2387,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="16">
-      <c r="A15" s="29"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2335,7 +2397,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="16">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2347,7 +2409,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="16">
-      <c r="A17" s="29"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2359,7 +2421,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="16">
-      <c r="A18" s="29"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2372,7 +2434,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="16">
-      <c r="A19" s="29"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2385,7 +2447,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="16">
-      <c r="A20" s="29"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2976,21 +3038,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
     <col min="2" max="2" width="40.1640625" customWidth="1"/>
-    <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" ht="45">
       <c r="A1" s="22" t="s">
         <v>145</v>
       </c>
@@ -2998,32 +3062,38 @@
         <v>146</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="30" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="26" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="30" t="s">
+      <c r="D3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-    </row>
-    <row r="5" spans="1:4" ht="16">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" ht="16">
       <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
@@ -3031,10 +3101,10 @@
         <v>151</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
       <c r="A6" s="26" t="s">
         <v>51</v>
       </c>
@@ -3042,10 +3112,10 @@
         <v>106</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="26" t="s">
         <v>49</v>
       </c>
@@ -3053,10 +3123,10 @@
         <v>152</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="26" t="s">
         <v>74</v>
       </c>
@@ -3064,10 +3134,10 @@
         <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="20" t="s">
         <v>75</v>
       </c>
@@ -3075,14 +3145,14 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="16" customFormat="1">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:5" s="16" customFormat="1">
+      <c r="A10" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
         <v>156</v>
       </c>
@@ -3090,14 +3160,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="16" customFormat="1">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:5" s="16" customFormat="1">
+      <c r="A12" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
         <v>159</v>
       </c>
@@ -3105,7 +3175,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="20" t="s">
         <v>161</v>
       </c>
@@ -3113,7 +3183,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="20" t="s">
         <v>163</v>
       </c>
@@ -3121,7 +3191,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="20" t="s">
         <v>165</v>
       </c>
@@ -3129,7 +3199,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
         <v>167</v>
       </c>
@@ -3137,22 +3207,28 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="16" customFormat="1">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:5" s="16" customFormat="1">
+      <c r="A18" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="20" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="20" t="s">
         <v>171</v>
       </c>
@@ -3160,7 +3236,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21" s="20" t="s">
         <v>172</v>
       </c>
@@ -3168,7 +3244,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="A22" s="20" t="s">
         <v>57</v>
       </c>
@@ -3176,153 +3252,156 @@
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="20" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="20" t="s">
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="16" customFormat="1">
+      <c r="A25" s="33" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" s="16" customFormat="1">
-      <c r="A24" s="30" t="s">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="20" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="20" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="20" t="s">
+      <c r="B27" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="20" t="s">
+      <c r="B28" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B27" s="20" t="s">
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="20" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="20" t="s">
+      <c r="B29" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="B28" s="20" t="s">
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="20" t="s">
+      <c r="B30" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="20" t="s">
+    </row>
+    <row r="31" spans="1:5" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="A31" s="33" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" s="16" customFormat="1" ht="18" customHeight="1">
-      <c r="A30" s="30" t="s">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="20" t="s">
+      <c r="B32" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="20" t="s">
-        <v>43</v>
+        <v>186</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="B34" s="20" t="s">
+    </row>
+    <row r="36" spans="1:4" s="16" customFormat="1">
+      <c r="A36" s="33" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="16" customFormat="1">
-      <c r="A35" s="30" t="s">
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" ht="16">
+      <c r="A37" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-    </row>
-    <row r="36" spans="1:4" ht="16">
-      <c r="A36" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>96</v>
+      <c r="D37" s="28" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="20" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>149</v>
+        <v>197</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="20" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>149</v>
@@ -3330,195 +3409,212 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="20" t="s">
-        <v>202</v>
+        <v>72</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="16" customFormat="1">
+      <c r="A48" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="16" customFormat="1">
-      <c r="A47" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="19" t="s">
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="19" t="s">
+      <c r="B49" s="21"/>
+      <c r="E49" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="19" customHeight="1">
+      <c r="A50" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16">
-      <c r="A50" s="27" t="s">
+      <c r="B50" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="F50" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16">
+      <c r="A51" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="16">
-      <c r="A51" s="27" t="s">
+      <c r="B51" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="16">
+      <c r="A52" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B52" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D51" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16">
-      <c r="A52" s="27" t="s">
+      <c r="D52" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="16">
+      <c r="A53" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B53" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16">
-      <c r="A53" s="27" t="s">
+      <c r="D53" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="16">
+      <c r="A54" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B54" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D53" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="19" t="s">
+      <c r="D54" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="19" t="s">
         <v>80</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="27" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="27" t="s">
+      <c r="B57" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" t="s">
         <v>242</v>
       </c>
-      <c r="D56" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="27" t="s">
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B58" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D57" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="19" t="s">
+      <c r="D58" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B59" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="27" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="27" t="s">
+      <c r="B60" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="D60" t="s">
         <v>242</v>
       </c>
-      <c r="D59" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="15" t="s">
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B61" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D61" t="s">
         <v>242</v>
       </c>
-      <c r="D60" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B61" s="15" t="s">
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B62" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D61" t="s">
-        <v>243</v>
+      <c r="D62" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A48:C48"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent"/>
-    <hyperlink ref="B33" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent"/>
-    <hyperlink ref="B43" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent"/>
-    <hyperlink ref="A48" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
-    <hyperlink ref="A50" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
+    <hyperlink ref="B34" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent"/>
+    <hyperlink ref="B44" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent"/>
+    <hyperlink ref="A49" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
+    <hyperlink ref="A51" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId6"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3551,36 +3647,36 @@
         <v>145</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" ht="288">
       <c r="A3" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="300">
       <c r="A4" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>217</v>
-      </c>
       <c r="C4" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
@@ -3588,30 +3684,30 @@
         <v>135</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1" t="s">
@@ -3630,11 +3726,11 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
     </row>
     <row r="12" spans="1:3" ht="16">
       <c r="A12" s="1" t="s">
@@ -3667,11 +3763,11 @@
       <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
+      <c r="A16" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
     </row>
     <row r="17" spans="1:3" ht="16">
       <c r="A17" s="1" t="s">
@@ -3702,18 +3798,18 @@
       <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="A21" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
     </row>
     <row r="22" spans="1:3" ht="16">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16">
@@ -3721,7 +3817,7 @@
         <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16">
@@ -3729,7 +3825,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16">
@@ -3737,25 +3833,25 @@
         <v>124</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
     </row>
     <row r="27" spans="1:3" ht="135">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="300">
@@ -3763,36 +3859,36 @@
         <v>13</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
       <c r="A29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
     </row>
     <row r="32" spans="1:3" ht="16">
       <c r="A32" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B32" s="17"/>
     </row>
     <row r="33" spans="1:3" ht="16">
       <c r="A33" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B33" t="s">
         <v>120</v>
@@ -3803,62 +3899,62 @@
         <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="30" t="s">
-        <v>219</v>
-      </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
     </row>
     <row r="37" spans="1:3" ht="195">
       <c r="A37" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B37" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="195">
       <c r="A38" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B38" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16">
       <c r="A39" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B39" s="17"/>
     </row>
     <row r="40" spans="1:3" ht="16">
       <c r="A40" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B40" s="17"/>
     </row>
     <row r="41" spans="1:3" ht="16">
       <c r="A41" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B41" s="17"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="B41" s="17"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
     </row>
     <row r="44" spans="1:3" ht="16">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
new owl statements included
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19660" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="253">
   <si>
     <t>Shape</t>
   </si>
@@ -971,9 +971,6 @@
   </si>
   <si>
     <t>owl:inverseOf</t>
-  </si>
-  <si>
-    <t>sh:inversePath/sh:equals</t>
   </si>
   <si>
     <t>dash:subSetOf</t>
@@ -1518,6 +1515,9 @@
   </si>
   <si>
     <t>sh:node apunta a un shape</t>
+  </si>
+  <si>
+    <t>sh:inversePath</t>
   </si>
 </sst>
 </file>
@@ -1633,7 +1633,7 @@
       <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1685,6 +1685,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1744,7 +1750,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1807,6 +1813,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2217,7 +2226,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2229,7 +2238,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16">
-      <c r="A3" s="32"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2250,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2263,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
-      <c r="A5" s="32"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2276,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="75">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,7 +2291,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2295,7 +2304,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2308,7 +2317,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2323,7 +2332,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2336,7 +2345,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2349,7 +2358,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="16">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2362,7 +2371,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="60">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2375,7 +2384,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="16">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="33" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2387,7 +2396,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="16">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2397,7 +2406,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="16">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2409,7 +2418,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="16">
-      <c r="A17" s="32"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2421,7 +2430,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="16">
-      <c r="A18" s="32"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2434,7 +2443,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="16">
-      <c r="A19" s="32"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2447,7 +2456,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="16">
-      <c r="A20" s="32"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -3040,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3062,15 +3071,15 @@
         <v>146</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="26" t="s">
@@ -3080,18 +3089,18 @@
         <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="1:5" ht="16">
       <c r="A5" s="26" t="s">
@@ -3101,7 +3110,7 @@
         <v>151</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16">
@@ -3112,7 +3121,7 @@
         <v>106</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
@@ -3123,7 +3132,7 @@
         <v>152</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3134,23 +3143,26 @@
         <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="26" t="s">
         <v>154</v>
       </c>
+      <c r="D9" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
@@ -3161,11 +3173,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="16" customFormat="1">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
@@ -3208,11 +3220,11 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="16" customFormat="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="26" t="s">
@@ -3222,10 +3234,10 @@
         <v>88</v>
       </c>
       <c r="D19" t="s">
+        <v>248</v>
+      </c>
+      <c r="E19" t="s">
         <v>249</v>
-      </c>
-      <c r="E19" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3241,7 +3253,7 @@
         <v>172</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3249,96 +3261,96 @@
         <v>57</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" t="s">
         <v>246</v>
       </c>
-      <c r="B24" s="26" t="s">
+    </row>
+    <row r="25" spans="1:5" s="16" customFormat="1">
+      <c r="A25" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="D24" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="16" customFormat="1">
-      <c r="A25" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>179</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="B30" s="20" t="s">
+    </row>
+    <row r="31" spans="1:5" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="A31" s="34" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" s="16" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>186</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3346,38 +3358,38 @@
         <v>43</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="B35" s="20" t="s">
+    </row>
+    <row r="36" spans="1:4" s="16" customFormat="1">
+      <c r="A36" s="34" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" s="16" customFormat="1">
-      <c r="A36" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
     </row>
     <row r="37" spans="1:4" ht="16">
       <c r="A37" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>96</v>
@@ -3385,18 +3397,18 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="20" t="s">
         <v>195</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>197</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3409,7 +3421,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>149</v>
@@ -3420,31 +3432,31 @@
         <v>72</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" s="20" t="s">
         <v>201</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="16" customFormat="1">
-      <c r="A48" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
+      <c r="A48" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="19" t="s">
@@ -3452,7 +3464,7 @@
       </c>
       <c r="B49" s="21"/>
       <c r="E49" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="19" customHeight="1">
@@ -3460,16 +3472,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="F50" t="s">
         <v>251</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="F50" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16">
@@ -3477,10 +3489,10 @@
         <v>55</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="16">
@@ -3491,7 +3503,7 @@
         <v>94</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="16">
@@ -3502,7 +3514,7 @@
         <v>78</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="16">
@@ -3513,7 +3525,7 @@
         <v>79</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3537,10 +3549,10 @@
         <v>60</v>
       </c>
       <c r="B57" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D57" t="s">
         <v>241</v>
-      </c>
-      <c r="D57" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3551,7 +3563,7 @@
         <v>83</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3567,10 +3579,10 @@
         <v>69</v>
       </c>
       <c r="B60" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D60" t="s">
         <v>241</v>
-      </c>
-      <c r="D60" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3578,21 +3590,21 @@
         <v>70</v>
       </c>
       <c r="B61" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D61" t="s">
         <v>241</v>
-      </c>
-      <c r="D61" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B62" s="15" t="s">
         <v>83</v>
       </c>
       <c r="D62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3647,36 +3659,36 @@
         <v>145</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:3" ht="288">
       <c r="A3" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="300">
       <c r="A4" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>216</v>
-      </c>
       <c r="C4" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
@@ -3684,30 +3696,30 @@
         <v>135</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1" t="s">
@@ -3726,11 +3738,11 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="A11" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:3" ht="16">
       <c r="A12" s="1" t="s">
@@ -3763,11 +3775,11 @@
       <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="A16" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:3" ht="16">
       <c r="A17" s="1" t="s">
@@ -3798,18 +3810,18 @@
       <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
+      <c r="A21" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
     </row>
     <row r="22" spans="1:3" ht="16">
       <c r="A22" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16">
@@ -3817,7 +3829,7 @@
         <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16">
@@ -3825,7 +3837,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16">
@@ -3833,25 +3845,25 @@
         <v>124</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
+      <c r="A26" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:3" ht="135">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="300">
@@ -3859,36 +3871,36 @@
         <v>13</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
       <c r="A29" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="B29" s="18" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="32" spans="1:3" ht="16">
       <c r="A32" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B32" s="17"/>
     </row>
     <row r="33" spans="1:3" ht="16">
       <c r="A33" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
         <v>120</v>
@@ -3899,62 +3911,62 @@
         <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
+      <c r="A36" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
     </row>
     <row r="37" spans="1:3" ht="195">
       <c r="A37" s="18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B37" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="195">
       <c r="A38" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B38" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16">
       <c r="A39" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B39" s="17"/>
     </row>
     <row r="40" spans="1:3" ht="16">
       <c r="A40" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B40" s="17"/>
     </row>
     <row r="41" spans="1:3" ht="16">
       <c r="A41" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B41" s="17"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="B41" s="17"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
     </row>
     <row r="44" spans="1:3" ht="16">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
new shacl tests validated
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19660" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="35200" windowHeight="19600" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -3049,8 +3049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3299,10 +3299,10 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3388,10 +3388,10 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="26" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new shacl tests validaded, new owl coverage included
</commit_message>
<xml_diff>
--- a/Shaper.xlsx
+++ b/Shaper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="35200" windowHeight="19600" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35500" windowHeight="17540" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SHAPE - ONTO" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <author>tc={55D55B28-10D5-458C-8AAA-BD5E74C44BC9}</author>
   </authors>
   <commentList>
-    <comment ref="A26" authorId="0">
+    <comment ref="A30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="1">
+    <comment ref="A37" authorId="1">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="256">
   <si>
     <t>Shape</t>
   </si>
@@ -1458,12 +1458,6 @@
     <t>RDFSchemaFeaturesTest</t>
   </si>
   <si>
-    <t xml:space="preserve">En este test si una clase esta definida como rdf:Property no se generará ninguna de estas restricciones </t>
-  </si>
-  <si>
-    <t>Comentar esto del domain</t>
-  </si>
-  <si>
     <t>owl:propertyChainAxiom</t>
   </si>
   <si>
@@ -1514,17 +1508,200 @@
     </r>
   </si>
   <si>
-    <t>sh:node apunta a un shape</t>
-  </si>
-  <si>
     <t>sh:inversePath</t>
+  </si>
+  <si>
+    <r>
+      <t>sh:maxExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:maxExclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:maxInclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:maxInclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>owl:onDatatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>owl:withRestrictions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>xsd:minInclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sh:minInclusive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> etc</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1632,6 +1809,11 @@
       <color rgb="FF24292E"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1684,14 +1866,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FF9BBB59"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1713,7 +1895,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1749,8 +1931,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1806,16 +1992,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1827,8 +2010,14 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
@@ -1863,6 +2052,10 @@
     <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2226,7 +2419,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2238,7 +2431,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="16">
-      <c r="A3" s="33"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2250,7 +2443,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="16">
-      <c r="A4" s="33"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2456,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16">
-      <c r="A5" s="33"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2276,7 +2469,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="75">
-      <c r="A6" s="33"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2291,7 +2484,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="16">
-      <c r="A7" s="33"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2304,7 +2497,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16">
-      <c r="A8" s="33"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2317,7 +2510,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2332,7 +2525,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="16">
-      <c r="A10" s="33"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2345,7 +2538,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="16">
-      <c r="A11" s="33"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2358,7 +2551,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="16">
-      <c r="A12" s="33"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2371,7 +2564,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="60">
-      <c r="A13" s="33"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2384,7 +2577,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="16">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2396,7 +2589,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="16">
-      <c r="A15" s="33"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2406,7 +2599,7 @@
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="16">
-      <c r="A16" s="33"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2418,7 +2611,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="16">
-      <c r="A17" s="33"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2430,7 +2623,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="16">
-      <c r="A18" s="33"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2636,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="16">
-      <c r="A19" s="33"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2456,7 +2649,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="16">
-      <c r="A20" s="33"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
@@ -3047,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3059,7 +3252,7 @@
     <col min="2" max="2" width="40.1640625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3075,11 +3268,11 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="26" t="s">
@@ -3092,15 +3285,15 @@
         <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="16">
       <c r="A5" s="26" t="s">
@@ -3158,475 +3351,511 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="26" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="16" customFormat="1">
-      <c r="A12" s="34" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="16" customFormat="1">
+      <c r="A15" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="20" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B16" s="26" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="20" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B17" s="26" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="20" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B18" s="26" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="16" customFormat="1">
-      <c r="A18" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="26" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" t="s">
-        <v>248</v>
-      </c>
-      <c r="E19" t="s">
-        <v>249</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="16" customFormat="1">
+      <c r="A21" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B23" s="20" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="26" t="s">
-        <v>245</v>
+        <v>75</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="D24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="16" customFormat="1">
-      <c r="A25" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="16" customFormat="1">
+      <c r="A29" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B30" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="26" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B32" s="26" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="32" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="16" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="20" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="20" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="16" customFormat="1">
-      <c r="A36" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-    </row>
-    <row r="37" spans="1:4" ht="16">
-      <c r="A37" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>236</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="A36" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>96</v>
+      <c r="A38" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="20" t="s">
-        <v>194</v>
+        <v>43</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="20" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>149</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="16" customFormat="1">
+      <c r="A41" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+    </row>
+    <row r="42" spans="1:4" ht="16">
+      <c r="A42" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>199</v>
+      <c r="A43" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="20" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B50" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="16" customFormat="1">
-      <c r="A48" s="34" t="s">
+    <row r="53" spans="1:5" s="16" customFormat="1">
+      <c r="A53" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="19" t="s">
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="E49" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="19" customHeight="1">
-      <c r="A50" s="30" t="s">
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="1:5" ht="19" customHeight="1">
+      <c r="A55" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="30" t="s">
-        <v>250</v>
-      </c>
-      <c r="D50" s="28" t="s">
+      <c r="B55" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="E50" s="29" t="s">
-        <v>242</v>
-      </c>
-      <c r="F50" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="16">
-      <c r="A51" s="30" t="s">
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="1:5" ht="16">
+      <c r="A56" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B56" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="D51" s="28" t="s">
+      <c r="D56" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16">
-      <c r="A52" s="27" t="s">
+    <row r="57" spans="1:5" ht="16">
+      <c r="A57" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B57" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D57" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16">
-      <c r="A53" s="27" t="s">
+    <row r="58" spans="1:5" ht="16">
+      <c r="A58" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B58" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D58" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16">
-      <c r="A54" s="27" t="s">
+    <row r="59" spans="1:5" ht="16">
+      <c r="A59" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B59" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D59" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="19" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B60" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="19" t="s">
+    <row r="61" spans="1:5">
+      <c r="A61" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B61" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="27" t="s">
+    <row r="62" spans="1:5">
+      <c r="A62" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B62" s="27" t="s">
         <v>240</v>
-      </c>
-      <c r="D57" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D58" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="D60" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="D61" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="D62" t="s">
         <v>241</v>
       </c>
     </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D63" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D64" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D66" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A53:C53"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent"/>
-    <hyperlink ref="B34" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent"/>
-    <hyperlink ref="B44" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent"/>
-    <hyperlink ref="A49" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
-    <hyperlink ref="A51" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
+    <hyperlink ref="B26" r:id="rId1" location="SubSetOfConstraintComponent" display="http://datashapes.org/constraints.html - SubSetOfConstraintComponent"/>
+    <hyperlink ref="B39" r:id="rId2" location="HasValueWithClassConstraintComponent" display="http://datashapes.org/constraints.html - HasValueWithClassConstraintComponent"/>
+    <hyperlink ref="B49" r:id="rId3" location="PrimaryKeyConstraintComponent" display="http://datashapes.org/constraints.html - PrimaryKeyConstraintComponent"/>
+    <hyperlink ref="A54" r:id="rId4" location="ch_domain" display="https://www.w3.org/TR/rdf-schema/ - ch_domain"/>
+    <hyperlink ref="A56" r:id="rId5" location="ch_comment" display="https://www.w3.org/TR/rdf-schema/ - ch_comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId6"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3663,11 +3892,11 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" ht="288">
       <c r="A3" s="23" t="s">
@@ -3700,11 +3929,11 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
     </row>
     <row r="7" spans="1:3" ht="16">
       <c r="A7" s="1" t="s">
@@ -3715,11 +3944,11 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
     </row>
     <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1" t="s">
@@ -3738,11 +3967,11 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
     </row>
     <row r="12" spans="1:3" ht="16">
       <c r="A12" s="1" t="s">
@@ -3775,11 +4004,11 @@
       <c r="B15" s="17"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
     </row>
     <row r="17" spans="1:3" ht="16">
       <c r="A17" s="1" t="s">
@@ -3810,11 +4039,11 @@
       <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
     </row>
     <row r="22" spans="1:3" ht="16">
       <c r="A22" s="1" t="s">
@@ -3849,11 +4078,11 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
     </row>
     <row r="27" spans="1:3" ht="135">
       <c r="A27" s="1" t="s">
@@ -3886,11 +4115,11 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
     </row>
     <row r="32" spans="1:3" ht="16">
       <c r="A32" s="18" t="s">
@@ -3915,11 +4144,11 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
     </row>
     <row r="37" spans="1:3" ht="195">
       <c r="A37" s="18" t="s">
@@ -3962,11 +4191,11 @@
       <c r="B41" s="17"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
     </row>
     <row r="44" spans="1:3" ht="16">
       <c r="A44" s="1" t="s">

</xml_diff>